<commit_message>
Updated Test020.2.xlsx step 18
</commit_message>
<xml_diff>
--- a/data/qa/QTP/Test020.2.xlsx
+++ b/data/qa/QTP/Test020.2.xlsx
@@ -72,9 +72,6 @@
     <t>Click on Create New List in left menu</t>
   </si>
   <si>
-    <t>Manage List page loaded with message "Must be registered to use this feature."</t>
-  </si>
-  <si>
     <t>In Public Studies drop-down menu a the top, select "QA Test Study - Public"</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>Under section 3), in Available Queries and Lists box, verify that all items contain either "[Q]-qa3inves …", "[SL]-qa3inves …",  or "[SL-G]-Global …"</t>
+  </si>
+  <si>
+    <t>Manage List page loaded</t>
   </si>
 </sst>
 </file>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -669,10 +669,10 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -698,13 +698,13 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -712,10 +712,10 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
         <v>49</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -723,7 +723,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -734,7 +734,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -745,7 +745,7 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -767,7 +767,7 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -778,7 +778,7 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -789,10 +789,10 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
         <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -800,7 +800,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -811,7 +811,7 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -822,7 +822,7 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -844,10 +844,10 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
         <v>51</v>
-      </c>
-      <c r="H16" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="6:8">
@@ -855,10 +855,10 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="6:8">
@@ -866,10 +866,10 @@
         <v>17</v>
       </c>
       <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
         <v>21</v>
-      </c>
-      <c r="H18" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="19" spans="6:8">
@@ -879,8 +879,8 @@
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="H19" t="s">
-        <v>18</v>
+      <c r="H19" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="6:8">
@@ -888,10 +888,10 @@
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="6:8">
@@ -899,10 +899,10 @@
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="6:8">
@@ -910,7 +910,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>15</v>
@@ -921,10 +921,10 @@
         <v>22</v>
       </c>
       <c r="G23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" t="s">
         <v>57</v>
-      </c>
-      <c r="H23" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="24" spans="6:8">
@@ -932,10 +932,10 @@
         <v>23</v>
       </c>
       <c r="G24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" t="s">
         <v>59</v>
-      </c>
-      <c r="H24" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="6:8">
@@ -943,10 +943,10 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="6:8">
@@ -954,7 +954,7 @@
         <v>25</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>15</v>
@@ -965,10 +965,10 @@
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="6:8">
@@ -976,7 +976,7 @@
         <v>27</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>15</v>
@@ -987,10 +987,10 @@
         <v>28</v>
       </c>
       <c r="G29" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" t="s">
         <v>61</v>
-      </c>
-      <c r="H29" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="6:8">
@@ -998,10 +998,10 @@
         <v>29</v>
       </c>
       <c r="G30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="6:8">
@@ -1009,7 +1009,7 @@
         <v>30</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>15</v>
@@ -1020,10 +1020,10 @@
         <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="6:8">
@@ -1031,7 +1031,7 @@
         <v>32</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>15</v>
@@ -1042,10 +1042,10 @@
         <v>33</v>
       </c>
       <c r="G34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" t="s">
         <v>23</v>
-      </c>
-      <c r="H34" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="35" spans="6:8">
@@ -1053,10 +1053,10 @@
         <v>34</v>
       </c>
       <c r="G35" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" t="s">
         <v>27</v>
-      </c>
-      <c r="H35" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="36" spans="6:8">
@@ -1064,7 +1064,7 @@
         <v>35</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>15</v>
@@ -1075,10 +1075,10 @@
         <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="6:8">
@@ -1086,10 +1086,10 @@
         <v>37</v>
       </c>
       <c r="G38" t="s">
+        <v>66</v>
+      </c>
+      <c r="H38" t="s">
         <v>67</v>
-      </c>
-      <c r="H38" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="39" spans="6:8">
@@ -1097,7 +1097,7 @@
         <v>38</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>15</v>
@@ -1108,10 +1108,10 @@
         <v>39</v>
       </c>
       <c r="G40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="6:8">
@@ -1119,7 +1119,7 @@
         <v>40</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>15</v>
@@ -1130,10 +1130,10 @@
         <v>41</v>
       </c>
       <c r="G42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="6:8">
@@ -1141,10 +1141,10 @@
         <v>42</v>
       </c>
       <c r="G43" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" t="s">
         <v>34</v>
-      </c>
-      <c r="H43" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="44" spans="6:8">
@@ -1152,10 +1152,10 @@
         <v>43</v>
       </c>
       <c r="G44" t="s">
+        <v>35</v>
+      </c>
+      <c r="H44" t="s">
         <v>36</v>
-      </c>
-      <c r="H44" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="45" spans="6:8">
@@ -1163,10 +1163,10 @@
         <v>44</v>
       </c>
       <c r="G45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" t="s">
         <v>38</v>
-      </c>
-      <c r="H45" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="46" spans="6:8">
@@ -1174,10 +1174,10 @@
         <v>45</v>
       </c>
       <c r="G46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Test 20.2 and 21
</commit_message>
<xml_diff>
--- a/data/qa/QTP/Test020.2.xlsx
+++ b/data/qa/QTP/Test020.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="870" windowWidth="25005" windowHeight="11955"/>
+    <workbookView xWindow="-105" yWindow="75" windowWidth="25005" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="TST001" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
   <si>
     <t>Expected Result</t>
   </si>
@@ -72,30 +72,12 @@
     <t>Click on Create New List in left menu</t>
   </si>
   <si>
-    <t>In Public Studies drop-down menu a the top, select "QA Test Study - Public"</t>
-  </si>
-  <si>
-    <t>Wecome to QA Test Study -Public page loaded</t>
-  </si>
-  <si>
-    <t>Click on Search QA Test Study - Public in left menu</t>
-  </si>
-  <si>
-    <t>Search QA Test Study - Public page loaded</t>
-  </si>
-  <si>
     <t>Click on KM Plot in left menu</t>
   </si>
   <si>
     <t>Kaplan-Meier Survival Plots page loaded</t>
   </si>
   <si>
-    <t>Verify that in Public Studies drop-down menu, the following studies are present: qa1adminpub, qa2adminpub, qa1managpub, qa2managpub</t>
-  </si>
-  <si>
-    <t>Verify that in Public Studies drop-down menu, the following studies are not present: qa1adminpri, qa2adminpri, qa1managpri, qa2managpri</t>
-  </si>
-  <si>
     <t>Click on tab For Queries and Saved Lists</t>
   </si>
   <si>
@@ -165,9 +147,6 @@
     <t>In My Studies drop-down menu a the top, select "-- Please Select --"</t>
   </si>
   <si>
-    <t>Wecome to caIntegrator page loaded</t>
-  </si>
-  <si>
     <t>Click on Study Log: View link</t>
   </si>
   <si>
@@ -262,13 +241,31 @@
   </si>
   <si>
     <t>Manage List page loaded</t>
+  </si>
+  <si>
+    <t>Verify that in My Studies drop-down menu, the following studies are present: qa1adminpub, qa2adminpub, qa1managpub, qa2managpub</t>
+  </si>
+  <si>
+    <t>Verify that in My Studies drop-down menu, the following studies are not present: qa1adminpri, qa2adminpri, qa1managpri, qa2managpri</t>
+  </si>
+  <si>
+    <t>In My Studies drop-down menu a the top, select "QA Test Study - QA3 Group"</t>
+  </si>
+  <si>
+    <t>Welcome to QA Test Study -QA3 Group page loaded</t>
+  </si>
+  <si>
+    <t>Click on Search QA Test Study - QA3 Group in left menu</t>
+  </si>
+  <si>
+    <t>Search QA Test Study - QA3 Group page loaded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +284,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -312,11 +316,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,7 +619,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -669,16 +674,16 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2">
-        <v>40667</v>
+        <v>40669</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -698,13 +703,13 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -712,10 +717,10 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -723,7 +728,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -734,7 +739,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -745,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -767,7 +772,7 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -778,7 +783,7 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -788,11 +793,11 @@
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
+      <c r="G11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -800,7 +805,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -811,7 +816,7 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -822,7 +827,7 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -844,10 +849,10 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="6:8">
@@ -855,21 +860,21 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="6:8">
       <c r="F18">
         <v>17</v>
       </c>
-      <c r="G18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" t="s">
-        <v>21</v>
+      <c r="G18" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="6:8">
@@ -880,7 +885,7 @@
         <v>17</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="6:8">
@@ -888,10 +893,10 @@
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H20" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="6:8">
@@ -899,10 +904,10 @@
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="6:8">
@@ -910,7 +915,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>15</v>
@@ -921,10 +926,10 @@
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H23" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="6:8">
@@ -932,10 +937,10 @@
         <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H24" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="6:8">
@@ -943,10 +948,10 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="6:8">
@@ -954,7 +959,7 @@
         <v>25</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>15</v>
@@ -965,10 +970,10 @@
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="6:8">
@@ -976,7 +981,7 @@
         <v>27</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>15</v>
@@ -987,10 +992,10 @@
         <v>28</v>
       </c>
       <c r="G29" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H29" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="6:8">
@@ -998,10 +1003,10 @@
         <v>29</v>
       </c>
       <c r="G30" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="6:8">
@@ -1009,7 +1014,7 @@
         <v>30</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>15</v>
@@ -1020,10 +1025,10 @@
         <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="6:8">
@@ -1031,7 +1036,7 @@
         <v>32</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>15</v>
@@ -1042,10 +1047,10 @@
         <v>33</v>
       </c>
       <c r="G34" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H34" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="6:8">
@@ -1053,10 +1058,10 @@
         <v>34</v>
       </c>
       <c r="G35" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H35" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="6:8">
@@ -1064,7 +1069,7 @@
         <v>35</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>15</v>
@@ -1075,10 +1080,10 @@
         <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H37" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="6:8">
@@ -1086,10 +1091,10 @@
         <v>37</v>
       </c>
       <c r="G38" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="H38" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="6:8">
@@ -1097,7 +1102,7 @@
         <v>38</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>15</v>
@@ -1108,10 +1113,10 @@
         <v>39</v>
       </c>
       <c r="G40" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H40" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="6:8">
@@ -1119,7 +1124,7 @@
         <v>40</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>15</v>
@@ -1130,10 +1135,10 @@
         <v>41</v>
       </c>
       <c r="G42" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H42" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="6:8">
@@ -1141,10 +1146,10 @@
         <v>42</v>
       </c>
       <c r="G43" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H43" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="6:8">
@@ -1152,10 +1157,10 @@
         <v>43</v>
       </c>
       <c r="G44" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H44" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="6:8">
@@ -1163,10 +1168,10 @@
         <v>44</v>
       </c>
       <c r="G45" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H45" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="6:8">
@@ -1174,10 +1179,10 @@
         <v>45</v>
       </c>
       <c r="G46" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H46" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>